<commit_message>
Added supplemental analysis on patients who filled script on the day of surgery.
</commit_message>
<xml_diff>
--- a/tables_for_paper.xlsx
+++ b/tables_for_paper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpishar\Desktop\eoa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpish\Documents\Research\Ortho\eoa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665849F3-A534-474E-AEE0-28152F58FED2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5FC786-3BE6-4B36-B611-A4F164AC3056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{B3DBD4D2-3816-4F19-905B-1249A3A8CC5C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{B3DBD4D2-3816-4F19-905B-1249A3A8CC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Elix" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId8"/>
+    <sheet name="arthritis_type" sheetId="7" r:id="rId8"/>
     <sheet name="Sheet7" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -28,12 +28,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
   <si>
     <t>Table: Descriptive statistics</t>
   </si>
@@ -548,6 +559,12 @@
       </rPr>
       <t>Mean (SD)</t>
     </r>
+  </si>
+  <si>
+    <t>Unspecified</t>
+  </si>
+  <si>
+    <t>Primary OA</t>
   </si>
 </sst>
 </file>
@@ -814,7 +831,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -829,7 +846,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -846,7 +863,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -880,12 +897,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -906,6 +923,51 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,51 +990,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -993,9 +1011,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1033,7 +1051,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1139,7 +1157,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1281,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1295,139 +1313,139 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="58"/>
-    <col min="3" max="3" width="48.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="2" width="9.1796875" style="47"/>
+    <col min="3" max="3" width="48.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="47"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="56" t="s">
+    <row r="4" spans="3:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="57"/>
-    </row>
-    <row r="5" spans="3:4" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="49"/>
-      <c r="D5" s="50" t="s">
+      <c r="D4" s="54"/>
+    </row>
+    <row r="5" spans="3:4" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="51" t="s">
+    <row r="6" spans="3:4" ht="13" x14ac:dyDescent="0.25">
+      <c r="C6" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="51" t="s">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="51" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C9" s="51" t="s">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="51" t="s">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="51" t="s">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="51" t="s">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="51" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="51" t="s">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="51" t="s">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="51" t="s">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="51" t="s">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="51" t="s">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="53" t="s">
+    <row r="19" spans="3:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:4" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C20" s="55" t="s">
         <v>31</v>
       </c>
@@ -1447,573 +1465,573 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9421064-70D7-4334-B25B-96DFE06AACC1}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H22" activeCellId="2" sqref="D22 F22 H22"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="59"/>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-    </row>
-    <row r="6" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="61" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+    </row>
+    <row r="6" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62" t="s">
+      <c r="D6" s="56"/>
+      <c r="E6" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62" t="s">
+      <c r="F6" s="57"/>
+      <c r="G6" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
-      <c r="B7" s="63" t="s">
+      <c r="H6" s="57"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="48"/>
+      <c r="B7" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="65">
+      <c r="I7" s="51"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="48"/>
+      <c r="B8" s="52">
         <v>2009</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="52">
         <v>39820</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="52">
         <v>0.84</v>
       </c>
-      <c r="E8" s="65">
+      <c r="E8" s="52">
         <v>28296</v>
       </c>
-      <c r="F8" s="65">
+      <c r="F8" s="52">
         <v>1.01</v>
       </c>
-      <c r="G8" s="65">
+      <c r="G8" s="52">
         <v>68116</v>
       </c>
-      <c r="H8" s="65">
+      <c r="H8" s="52">
         <v>0.91</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="65">
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="48"/>
+      <c r="B9" s="52">
         <v>2010</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="52">
         <v>38271</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="52">
         <v>0.99</v>
       </c>
-      <c r="E9" s="65">
+      <c r="E9" s="52">
         <v>31947</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="52">
         <v>1.05</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="52">
         <v>70218</v>
       </c>
-      <c r="H9" s="65">
+      <c r="H9" s="52">
         <v>1.02</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="65">
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="48"/>
+      <c r="B10" s="52">
         <v>2011</v>
       </c>
-      <c r="C10" s="65">
+      <c r="C10" s="52">
         <v>40555</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="52">
         <v>0.86</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="52">
         <v>35917</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="52">
         <v>0.98</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="52">
         <v>76472</v>
       </c>
-      <c r="H10" s="65">
+      <c r="H10" s="52">
         <v>0.92</v>
       </c>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="65">
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="48"/>
+      <c r="B11" s="52">
         <v>2012</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="52">
         <v>39097</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="52">
         <v>0.98</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="52">
         <v>36171</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="52">
         <v>0.97</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="52">
         <v>75268</v>
       </c>
-      <c r="H11" s="65">
+      <c r="H11" s="52">
         <v>0.98</v>
       </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="65">
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="48"/>
+      <c r="B12" s="52">
         <v>2013</v>
       </c>
-      <c r="C12" s="65">
+      <c r="C12" s="52">
         <v>32369</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="52">
         <v>0.93</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="52">
         <v>31559</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="52">
         <v>1.03</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="52">
         <v>63928</v>
       </c>
-      <c r="H12" s="65">
+      <c r="H12" s="52">
         <v>0.98</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="65">
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="48"/>
+      <c r="B13" s="52">
         <v>2014</v>
       </c>
-      <c r="C13" s="65">
+      <c r="C13" s="52">
         <v>31859</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="52">
         <v>0.91</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="52">
         <v>33497</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="52">
         <v>1.04</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="52">
         <v>65356</v>
       </c>
-      <c r="H13" s="65">
+      <c r="H13" s="52">
         <v>0.98</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="65">
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="48"/>
+      <c r="B14" s="52">
         <v>2015</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="52">
         <v>19825</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="52">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="52">
         <v>23102</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="52">
         <v>1.22</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="52">
         <v>42927</v>
       </c>
-      <c r="H14" s="65">
+      <c r="H14" s="52">
         <v>1.1599999999999999</v>
       </c>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="65">
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="48"/>
+      <c r="B15" s="52">
         <v>2016</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="52">
         <v>22723</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="52">
         <v>1.17</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="52">
         <v>28288</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="52">
         <v>1.5</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="52">
         <v>51011</v>
       </c>
-      <c r="H15" s="65">
+      <c r="H15" s="52">
         <v>1.35</v>
       </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="65">
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="48"/>
+      <c r="B16" s="52">
         <v>2017</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="52">
         <v>18837</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="52">
         <v>1.39</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="52">
         <v>24870</v>
       </c>
-      <c r="F16" s="65">
+      <c r="F16" s="52">
         <v>1.86</v>
       </c>
-      <c r="G16" s="65">
+      <c r="G16" s="52">
         <v>43707</v>
       </c>
-      <c r="H16" s="65">
+      <c r="H16" s="52">
         <v>1.66</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="65">
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="48"/>
+      <c r="B17" s="52">
         <v>2018</v>
       </c>
-      <c r="C17" s="65">
+      <c r="C17" s="52">
         <v>18013</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="52">
         <v>2.02</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="52">
         <v>23805</v>
       </c>
-      <c r="F17" s="65">
+      <c r="F17" s="52">
         <v>2.66</v>
       </c>
-      <c r="G17" s="65">
+      <c r="G17" s="52">
         <v>41818</v>
       </c>
-      <c r="H17" s="65">
+      <c r="H17" s="52">
         <v>2.38</v>
       </c>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="65">
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="48"/>
+      <c r="B18" s="52">
         <v>2019</v>
       </c>
-      <c r="C18" s="65">
+      <c r="C18" s="52">
         <v>13447</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="52">
         <v>2.75</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="52">
         <v>18780</v>
       </c>
-      <c r="F18" s="65">
+      <c r="F18" s="52">
         <v>3.78</v>
       </c>
-      <c r="G18" s="65">
+      <c r="G18" s="52">
         <v>32227</v>
       </c>
-      <c r="H18" s="65">
+      <c r="H18" s="52">
         <v>3.35</v>
       </c>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="65">
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="48"/>
+      <c r="B19" s="52">
         <v>2020</v>
       </c>
-      <c r="C19" s="65">
+      <c r="C19" s="52">
         <v>13184</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="52">
         <v>3.66</v>
       </c>
-      <c r="E19" s="65">
+      <c r="E19" s="52">
         <v>17182</v>
       </c>
-      <c r="F19" s="65">
+      <c r="F19" s="52">
         <v>5.28</v>
       </c>
-      <c r="G19" s="65">
+      <c r="G19" s="52">
         <v>30366</v>
       </c>
-      <c r="H19" s="65">
+      <c r="H19" s="52">
         <v>4.58</v>
       </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="65">
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="48"/>
+      <c r="B20" s="52">
         <v>2021</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="52">
         <v>14786</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="52">
         <v>5.31</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="52">
         <v>19878</v>
       </c>
-      <c r="F20" s="65">
+      <c r="F20" s="52">
         <v>7.67</v>
       </c>
-      <c r="G20" s="65">
+      <c r="G20" s="52">
         <v>34664</v>
       </c>
-      <c r="H20" s="65">
+      <c r="H20" s="52">
         <v>6.66</v>
       </c>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="65">
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="48"/>
+      <c r="B21" s="52">
         <v>2022</v>
       </c>
-      <c r="C21" s="65">
+      <c r="C21" s="52">
         <v>6838</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="52">
         <v>6.6</v>
       </c>
-      <c r="E21" s="65">
+      <c r="E21" s="52">
         <v>9296</v>
       </c>
-      <c r="F21" s="65">
+      <c r="F21" s="52">
         <v>8.9499999999999993</v>
       </c>
-      <c r="G21" s="65">
+      <c r="G21" s="52">
         <v>16134</v>
       </c>
-      <c r="H21" s="65">
+      <c r="H21" s="52">
         <v>7.95</v>
       </c>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59">
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48">
         <f>D21/D8 -1</f>
         <v>6.8571428571428568</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59">
-        <f t="shared" ref="E22:H22" si="0">F21/F8 -1</f>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48">
+        <f t="shared" ref="F22:H22" si="0">F21/F8 -1</f>
         <v>7.8613861386138613</v>
       </c>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59">
+      <c r="G22" s="48"/>
+      <c r="H22" s="48">
         <f t="shared" si="0"/>
         <v>7.7362637362637354</v>
       </c>
-      <c r="I22" s="59"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="59"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G28" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2034,13 +2052,13 @@
       <selection activeCell="G7" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="31" t="s">
         <v>163</v>
       </c>
@@ -2051,7 +2069,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>156</v>
       </c>
@@ -2062,7 +2080,7 @@
         <v>0.21887487999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>157</v>
       </c>
@@ -2073,7 +2091,7 @@
         <v>1.5831540000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="27" t="s">
         <v>158</v>
       </c>
@@ -2084,7 +2102,7 @@
         <v>0.40585612999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="27" t="s">
         <v>159</v>
       </c>
@@ -2095,7 +2113,7 @@
         <v>5.7869660000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>160</v>
       </c>
@@ -2106,7 +2124,7 @@
         <v>9.9677219999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="30" t="s">
         <v>161</v>
       </c>
@@ -2131,9 +2149,9 @@
       <selection activeCell="K43" sqref="H11:K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="8" spans="3:10" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="7" t="s">
         <v>35</v>
       </c>
@@ -2141,7 +2159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" ht="21.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C9" s="6">
         <v>2009</v>
       </c>
@@ -2149,7 +2167,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="6">
         <v>2010</v>
       </c>
@@ -2161,7 +2179,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="3:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" ht="21" x14ac:dyDescent="0.35">
       <c r="C11" s="6">
         <v>2011</v>
       </c>
@@ -2170,7 +2188,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="6">
         <v>2012</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="6">
         <v>2013</v>
       </c>
@@ -2192,7 +2210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="6">
         <v>2014</v>
       </c>
@@ -2203,7 +2221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="6">
         <v>2015</v>
       </c>
@@ -2214,7 +2232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="6">
         <v>2016</v>
       </c>
@@ -2225,7 +2243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="6">
         <v>2017</v>
       </c>
@@ -2236,7 +2254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="6">
         <v>2018</v>
       </c>
@@ -2247,7 +2265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="6">
         <v>2019</v>
       </c>
@@ -2258,7 +2276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="6">
         <v>2020</v>
       </c>
@@ -2269,7 +2287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="6">
         <v>2021</v>
       </c>
@@ -2280,7 +2298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="6">
         <v>2022</v>
       </c>
@@ -2291,107 +2309,107 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G24" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G25" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G26" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G27" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G28" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G29" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G30" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G31" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G32" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G33" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G34" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G35" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G36" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G37" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G38" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G39" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G40" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G41" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G42" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G43" s="3">
         <v>32</v>
       </c>
@@ -2410,13 +2428,13 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>47</v>
       </c>
@@ -2428,7 +2446,7 @@
         <v>0.70677410658624118</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>64</v>
       </c>
@@ -2440,7 +2458,7 @@
         <v>0.33066839648868596</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -2455,7 +2473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
         <v>52</v>
       </c>
@@ -2467,7 +2485,7 @@
         <v>0.24037505686509072</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -2479,7 +2497,7 @@
         <v>0.19707053517772799</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
         <v>43</v>
       </c>
@@ -2491,7 +2509,7 @@
         <v>0.18230246050333326</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
         <v>51</v>
       </c>
@@ -2503,7 +2521,7 @@
         <v>0.18086749451006162</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
         <v>72</v>
       </c>
@@ -2515,7 +2533,7 @@
         <v>0.17449720027182916</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
         <v>66</v>
       </c>
@@ -2527,7 +2545,7 @@
         <v>0.10694989694079853</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="8" t="s">
         <v>44</v>
       </c>
@@ -2539,7 +2557,7 @@
         <v>9.2066688008626649E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="8" t="s">
         <v>53</v>
       </c>
@@ -2551,7 +2569,7 @@
         <v>8.7132763839980226E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
         <v>62</v>
       </c>
@@ -2563,7 +2581,7 @@
         <v>8.0683841328143865E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
         <v>48</v>
       </c>
@@ -2575,7 +2593,7 @@
         <v>7.725087473954384E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
         <v>46</v>
       </c>
@@ -2587,7 +2605,7 @@
         <v>7.335035073826332E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
@@ -2599,7 +2617,7 @@
         <v>7.0504288049064043E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
         <v>68</v>
       </c>
@@ -2611,7 +2629,7 @@
         <v>5.8149820559047029E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
         <v>55</v>
       </c>
@@ -2623,7 +2641,7 @@
         <v>5.161805754466367E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
         <v>42</v>
       </c>
@@ -2635,7 +2653,7 @@
         <v>4.9403829196924515E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
         <v>63</v>
       </c>
@@ -2647,7 +2665,7 @@
         <v>4.0271716848354143E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
         <v>56</v>
       </c>
@@ -2659,7 +2677,7 @@
         <v>3.8721616597305296E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="8" t="s">
         <v>50</v>
       </c>
@@ -2671,7 +2689,7 @@
         <v>2.8835515267925844E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="8" t="s">
         <v>45</v>
       </c>
@@ -2683,7 +2701,7 @@
         <v>2.2310772635114263E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="8" t="s">
         <v>67</v>
       </c>
@@ -2695,7 +2713,7 @@
         <v>1.7765777605544417E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
         <v>70</v>
       </c>
@@ -2707,7 +2725,7 @@
         <v>1.5266521765991026E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
         <v>69</v>
       </c>
@@ -2719,7 +2737,7 @@
         <v>1.400004493044206E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="8" t="s">
         <v>65</v>
       </c>
@@ -2731,7 +2749,7 @@
         <v>1.3408928802098251E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
         <v>57</v>
       </c>
@@ -2743,7 +2761,7 @@
         <v>1.0043357876587309E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="8" t="s">
         <v>71</v>
       </c>
@@ -2755,7 +2773,7 @@
         <v>6.3885472303190621E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
@@ -2767,7 +2785,7 @@
         <v>5.777774033574273E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="8" t="s">
         <v>60</v>
       </c>
@@ -2779,7 +2797,7 @@
         <v>4.9128630239310767E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="8" t="s">
         <v>49</v>
       </c>
@@ -2791,7 +2809,7 @@
         <v>2.893801283887382E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="8" t="s">
         <v>58</v>
       </c>
@@ -2803,13 +2821,13 @@
         <v>7.7083789658135497E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A1:C33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C33">
     <sortCondition descending="1" ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2824,26 +2842,26 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-    </row>
-    <row r="7" spans="2:6" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+    <row r="6" spans="2:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+    </row>
+    <row r="7" spans="2:6" ht="20.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="60"/>
       <c r="C7" s="15" t="s">
         <v>75</v>
       </c>
@@ -2853,12 +2871,12 @@
       <c r="E7" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="62" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="44"/>
+    <row r="8" spans="2:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="61"/>
       <c r="C8" s="16" t="s">
         <v>76</v>
       </c>
@@ -2868,9 +2886,9 @@
       <c r="E8" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="46"/>
-    </row>
-    <row r="9" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="F8" s="63"/>
+    </row>
+    <row r="9" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
         <v>81</v>
       </c>
@@ -2887,7 +2905,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
         <v>85</v>
       </c>
@@ -2904,7 +2922,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>89</v>
       </c>
@@ -2921,7 +2939,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
         <v>93</v>
       </c>
@@ -2938,7 +2956,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
         <v>97</v>
       </c>
@@ -2955,7 +2973,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
         <v>102</v>
       </c>
@@ -2972,7 +2990,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
         <v>106</v>
       </c>
@@ -2989,7 +3007,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B16" s="17" t="s">
         <v>110</v>
       </c>
@@ -3006,7 +3024,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B17" s="17" t="s">
         <v>114</v>
       </c>
@@ -3023,7 +3041,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="20" x14ac:dyDescent="0.35">
       <c r="B18" s="17" t="s">
         <v>118</v>
       </c>
@@ -3040,7 +3058,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="19" t="s">
         <v>122</v>
       </c>
@@ -3057,7 +3075,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="F20" s="14"/>
     </row>
   </sheetData>
@@ -3078,26 +3096,26 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+    <row r="1" spans="1:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="41.25" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" s="23"/>
       <c r="B2" s="15" t="s">
         <v>75</v>
@@ -3113,7 +3131,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="24"/>
       <c r="B3" s="16" t="s">
         <v>76</v>
@@ -3127,7 +3145,7 @@
       <c r="E3" s="24"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
@@ -3145,7 +3163,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
@@ -3163,7 +3181,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="17" t="s">
         <v>6</v>
       </c>
@@ -3181,7 +3199,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="17" t="s">
         <v>29</v>
       </c>
@@ -3199,7 +3217,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
@@ -3217,7 +3235,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="17" t="s">
         <v>10</v>
       </c>
@@ -3235,7 +3253,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="17" t="s">
         <v>12</v>
       </c>
@@ -3253,7 +3271,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -3271,7 +3289,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
@@ -3289,7 +3307,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="17" t="s">
         <v>18</v>
       </c>
@@ -3307,7 +3325,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
@@ -3325,7 +3343,7 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
@@ -3343,7 +3361,7 @@
       </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="17" t="s">
         <v>24</v>
       </c>
@@ -3361,7 +3379,7 @@
       </c>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="17" t="s">
         <v>26</v>
       </c>
@@ -3379,7 +3397,7 @@
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A18" s="25"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3387,7 +3405,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3406,45 +3424,57 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4464D4A-37E4-4425-8740-6C871D1B96A5}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="35"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="64"/>
+      <c r="D1" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
+      <c r="E1" s="64"/>
+      <c r="F1" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48" t="s">
+      <c r="G1" s="64"/>
+      <c r="H1" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="48"/>
-    </row>
-    <row r="2" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I1" s="65"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+    </row>
+    <row r="2" spans="1:24" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="36" t="s">
         <v>35</v>
       </c>
@@ -3472,8 +3502,36 @@
       <c r="I2" s="37" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N2" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="T2" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="V2" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="W2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="X2" s="37"/>
+    </row>
+    <row r="3" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="5">
         <v>2009</v>
       </c>
@@ -3501,8 +3559,36 @@
       <c r="I3" s="39">
         <v>7.3600000000000002E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N3" s="5">
+        <v>2009</v>
+      </c>
+      <c r="O3" s="39">
+        <v>9.9699999999999997E-3</v>
+      </c>
+      <c r="P3" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="39">
+        <v>0</v>
+      </c>
+      <c r="R3" s="39">
+        <v>7.3600000000000002E-3</v>
+      </c>
+      <c r="T3" s="5">
+        <v>2009</v>
+      </c>
+      <c r="U3" s="39">
+        <v>9.9699999999999997E-3</v>
+      </c>
+      <c r="V3" s="39">
+        <v>0</v>
+      </c>
+      <c r="W3" s="39">
+        <v>0</v>
+      </c>
+      <c r="X3" s="39"/>
+    </row>
+    <row r="4" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="5">
         <v>2010</v>
       </c>
@@ -3530,8 +3616,36 @@
       <c r="I4" s="39">
         <v>9.8899999999999995E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N4" s="5">
+        <v>2010</v>
+      </c>
+      <c r="O4" s="39">
+        <v>1.03E-2</v>
+      </c>
+      <c r="P4" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="39">
+        <v>0</v>
+      </c>
+      <c r="R4" s="39">
+        <v>9.8899999999999995E-3</v>
+      </c>
+      <c r="T4" s="5">
+        <v>2010</v>
+      </c>
+      <c r="U4" s="39">
+        <v>1.03E-2</v>
+      </c>
+      <c r="V4" s="39">
+        <v>0</v>
+      </c>
+      <c r="W4" s="39">
+        <v>0</v>
+      </c>
+      <c r="X4" s="39"/>
+    </row>
+    <row r="5" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="5">
         <v>2011</v>
       </c>
@@ -3559,8 +3673,36 @@
       <c r="I5" s="39">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N5" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O5" s="39">
+        <v>8.8199999999999997E-3</v>
+      </c>
+      <c r="P5" s="39">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="Q5" s="39">
+        <v>0</v>
+      </c>
+      <c r="R5" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="T5" s="5">
+        <v>2011</v>
+      </c>
+      <c r="U5" s="39">
+        <v>8.8199999999999997E-3</v>
+      </c>
+      <c r="V5" s="39">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="W5" s="39">
+        <v>0</v>
+      </c>
+      <c r="X5" s="39"/>
+    </row>
+    <row r="6" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="5">
         <v>2012</v>
       </c>
@@ -3588,8 +3730,36 @@
       <c r="I6" s="39">
         <v>9.1699999999999993E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N6" s="5">
+        <v>2012</v>
+      </c>
+      <c r="O6" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="P6" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="39">
+        <v>1.2E-2</v>
+      </c>
+      <c r="R6" s="39">
+        <v>9.1699999999999993E-3</v>
+      </c>
+      <c r="T6" s="5">
+        <v>2012</v>
+      </c>
+      <c r="U6" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="V6" s="39">
+        <v>0</v>
+      </c>
+      <c r="W6" s="39">
+        <v>1.2E-2</v>
+      </c>
+      <c r="X6" s="39"/>
+    </row>
+    <row r="7" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="5">
         <v>2013</v>
       </c>
@@ -3617,8 +3787,36 @@
       <c r="I7" s="39">
         <v>9.9799999999999993E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N7" s="5">
+        <v>2013</v>
+      </c>
+      <c r="O7" s="39">
+        <v>9.7099999999999999E-3</v>
+      </c>
+      <c r="P7" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="39">
+        <v>0</v>
+      </c>
+      <c r="R7" s="39">
+        <v>9.9799999999999993E-3</v>
+      </c>
+      <c r="T7" s="5">
+        <v>2013</v>
+      </c>
+      <c r="U7" s="39">
+        <v>9.7099999999999999E-3</v>
+      </c>
+      <c r="V7" s="39">
+        <v>0</v>
+      </c>
+      <c r="W7" s="39">
+        <v>0</v>
+      </c>
+      <c r="X7" s="39"/>
+    </row>
+    <row r="8" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="5">
         <v>2014</v>
       </c>
@@ -3646,8 +3844,36 @@
       <c r="I8" s="39">
         <v>1.04E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N8" s="5">
+        <v>2014</v>
+      </c>
+      <c r="O8" s="39">
+        <v>9.4500000000000001E-3</v>
+      </c>
+      <c r="P8" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="39">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="R8" s="39">
+        <v>1.04E-2</v>
+      </c>
+      <c r="T8" s="5">
+        <v>2014</v>
+      </c>
+      <c r="U8" s="39">
+        <v>9.4500000000000001E-3</v>
+      </c>
+      <c r="V8" s="39">
+        <v>0</v>
+      </c>
+      <c r="W8" s="39">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="X8" s="39"/>
+    </row>
+    <row r="9" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="5">
         <v>2015</v>
       </c>
@@ -3675,8 +3901,36 @@
       <c r="I9" s="39">
         <v>1.18E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N9" s="5">
+        <v>2015</v>
+      </c>
+      <c r="O9" s="39">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="P9" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="39">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="R9" s="39">
+        <v>1.18E-2</v>
+      </c>
+      <c r="T9" s="5">
+        <v>2015</v>
+      </c>
+      <c r="U9" s="39">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="V9" s="39">
+        <v>0</v>
+      </c>
+      <c r="W9" s="39">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="X9" s="39"/>
+    </row>
+    <row r="10" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="5">
         <v>2016</v>
       </c>
@@ -3704,8 +3958,36 @@
       <c r="I10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N10" s="5">
+        <v>2016</v>
+      </c>
+      <c r="O10" s="39">
+        <v>1.35E-2</v>
+      </c>
+      <c r="P10" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="39">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5">
+        <v>2016</v>
+      </c>
+      <c r="U10" s="39">
+        <v>1.35E-2</v>
+      </c>
+      <c r="V10" s="39">
+        <v>0</v>
+      </c>
+      <c r="W10" s="39">
+        <v>0</v>
+      </c>
+      <c r="X10" s="5"/>
+    </row>
+    <row r="11" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="5">
         <v>2017</v>
       </c>
@@ -3733,8 +4015,36 @@
       <c r="I11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N11" s="5">
+        <v>2017</v>
+      </c>
+      <c r="O11" s="39">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="P11" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="39">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U11" s="39">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="V11" s="39">
+        <v>0</v>
+      </c>
+      <c r="W11" s="39">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="X11" s="5"/>
+    </row>
+    <row r="12" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="5">
         <v>2018</v>
       </c>
@@ -3762,8 +4072,36 @@
       <c r="I12" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N12" s="5">
+        <v>2018</v>
+      </c>
+      <c r="O12" s="39">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="P12" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="Q12" s="39">
+        <v>0</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0</v>
+      </c>
+      <c r="T12" s="5">
+        <v>2018</v>
+      </c>
+      <c r="U12" s="39">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="V12" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="W12" s="39">
+        <v>0</v>
+      </c>
+      <c r="X12" s="5"/>
+    </row>
+    <row r="13" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="5">
         <v>2019</v>
       </c>
@@ -3791,8 +4129,36 @@
       <c r="I13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N13" s="5">
+        <v>2019</v>
+      </c>
+      <c r="O13" s="39">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="P13" s="39">
+        <v>0.08</v>
+      </c>
+      <c r="Q13" s="39">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0</v>
+      </c>
+      <c r="T13" s="5">
+        <v>2019</v>
+      </c>
+      <c r="U13" s="39">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="V13" s="39">
+        <v>0.08</v>
+      </c>
+      <c r="W13" s="39">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="X13" s="5"/>
+    </row>
+    <row r="14" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="5">
         <v>2020</v>
       </c>
@@ -3820,8 +4186,36 @@
       <c r="I14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N14" s="5">
+        <v>2020</v>
+      </c>
+      <c r="O14" s="39">
+        <v>4.58E-2</v>
+      </c>
+      <c r="P14" s="39">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="Q14" s="39">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <v>2020</v>
+      </c>
+      <c r="U14" s="39">
+        <v>4.58E-2</v>
+      </c>
+      <c r="V14" s="39">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="W14" s="39">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="X14" s="5"/>
+    </row>
+    <row r="15" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="5">
         <v>2021</v>
       </c>
@@ -3849,8 +4243,36 @@
       <c r="I15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N15" s="5">
+        <v>2021</v>
+      </c>
+      <c r="O15" s="39">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="P15" s="39">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="Q15" s="39">
+        <v>0.19</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0</v>
+      </c>
+      <c r="T15" s="5">
+        <v>2021</v>
+      </c>
+      <c r="U15" s="39">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="V15" s="39">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="W15" s="39">
+        <v>0.19</v>
+      </c>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="16" spans="1:24" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="5">
         <v>2022</v>
       </c>
@@ -3878,8 +4300,36 @@
       <c r="I16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="N16" s="5">
+        <v>2022</v>
+      </c>
+      <c r="O16" s="39">
+        <v>7.9500000000000001E-2</v>
+      </c>
+      <c r="P16" s="39">
+        <v>0.182</v>
+      </c>
+      <c r="Q16" s="39">
+        <v>0.125</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0</v>
+      </c>
+      <c r="T16" s="5">
+        <v>2022</v>
+      </c>
+      <c r="U16" s="39">
+        <v>7.9500000000000001E-2</v>
+      </c>
+      <c r="V16" s="39">
+        <v>0.182</v>
+      </c>
+      <c r="W16" s="39">
+        <v>0.125</v>
+      </c>
+      <c r="X16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="35" t="s">
         <v>165</v>
       </c>
@@ -3904,10 +4354,10 @@
       </c>
       <c r="I17" s="35"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="I21" s="26"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23">
         <f>B17/SUM(B17,D17,F17,H17,)</f>
         <v>0.80039614126981229</v>
@@ -3916,13 +4366,44 @@
         <f>B17/712212</f>
         <v>0.80114347975041145</v>
       </c>
+      <c r="H23">
+        <f>H17/(H17+F17+D17+B17)</f>
+        <v>0.19820249496056122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <f>H17/(H17+F17+D17)</f>
+        <v>0.99297927515759732</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+    </row>
+    <row r="28" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28" s="37"/>
+    </row>
+    <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="A43" s="35"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3937,13 +4418,13 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="31" t="s">
         <v>163</v>
       </c>
@@ -3954,7 +4435,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>158</v>
       </c>
@@ -3965,7 +4446,7 @@
         <v>0.40585612999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>156</v>
       </c>
@@ -3976,7 +4457,7 @@
         <v>0.21887487999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="30" t="s">
         <v>161</v>
       </c>
@@ -3987,7 +4468,7 @@
         <v>0.20189056</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="27" t="s">
         <v>160</v>
       </c>
@@ -3998,7 +4479,7 @@
         <v>9.9677219999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>159</v>
       </c>
@@ -4009,7 +4490,7 @@
         <v>5.7869660000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="27" t="s">
         <v>157</v>
       </c>
@@ -4021,7 +4502,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C7">
     <sortCondition descending="1" ref="C2:C7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>